<commit_message>
[RC][Minor changes] Plotting windows and safety backup
Just minor changes and a safety backup to be up to date.
</commit_message>
<xml_diff>
--- a/SuspiciousPatternId/results/Book1.xlsx
+++ b/SuspiciousPatternId/results/Book1.xlsx
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinte/Documents/cheatersdemise/SuspiciousPatternId/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4331D2CC-9B26-ED4B-96BA-1B8B51D83250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58991677-AC83-EF4B-82F8-8EFFF1CA744B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{ED8BEE3F-D482-3F4C-A7CB-C740BA7E49C5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="10" sheetId="1" r:id="rId1"/>
+    <sheet name="20" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'10'!$A$1:$C$4</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'10'!$A$5:$C$5</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'10'!$A$5:$B$5</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'10'!$C$1:$C$4</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'10'!$C$5</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'10'!$A$5:$B$5</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'10'!$C$1:$C$4</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'10'!$C$5</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,12 +42,87 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>0.97 (+/- 0.10)</t>
-  </si>
-  <si>
-    <t>0.99 (+/- 0.05)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>0.99</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>0.98</t>
+  </si>
+  <si>
+    <t>Minutes</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>coll</t>
+  </si>
+  <si>
+    <t>harv</t>
+  </si>
+  <si>
+    <t>94.92%</t>
+  </si>
+  <si>
+    <t>5.07%</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>0.13</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
+    <t>0.22</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>90.03%</t>
+  </si>
+  <si>
+    <t>9.96%</t>
+  </si>
+  <si>
+    <t>68.91%</t>
+  </si>
+  <si>
+    <t>30.08%</t>
+  </si>
+  <si>
+    <t>56.60%</t>
+  </si>
+  <si>
+    <t>43.39%</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>pairs</t>
+  </si>
+  <si>
+    <t>user</t>
   </si>
 </sst>
 </file>
@@ -52,10 +138,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,9 +165,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,71 +488,330 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84766D11-EDB6-9144-AEF1-C289B749A806}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C1">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>92</v>
+      </c>
+      <c r="I2">
+        <v>53</v>
+      </c>
+      <c r="J2">
+        <f>H2/$L$2</f>
+        <v>2.7727546714888487E-2</v>
+      </c>
+      <c r="L2">
+        <v>3318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3">
+        <v>147</v>
+      </c>
+      <c r="I3">
+        <v>74</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J5" si="0">H3/$L$2</f>
+        <v>4.4303797468354431E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <v>437</v>
+      </c>
+      <c r="I4">
+        <v>271</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>0.13170584689572032</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="B5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>10</v>
-      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5">
+        <v>864</v>
+      </c>
+      <c r="I5">
+        <v>769</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0.2603978300180832</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC4D32B-D5D9-B84E-A4B2-1B873DDF310A}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.54049999999999998</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.45939999999999998</v>
+      </c>
+      <c r="H2">
+        <v>69</v>
+      </c>
+      <c r="I2">
+        <v>37</v>
+      </c>
+      <c r="J2">
+        <f>H2/$K$2</f>
+        <v>3.3061811212266409E-2</v>
+      </c>
+      <c r="K2">
+        <v>2087</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.55259999999999998</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.44729999999999998</v>
+      </c>
+      <c r="H3">
+        <v>71</v>
+      </c>
+      <c r="I3">
+        <v>38</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J5" si="0">H3/$K$2</f>
+        <v>3.4020124580737901E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.56810000000000005</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.43180000000000002</v>
+      </c>
+      <c r="H4">
+        <v>79</v>
+      </c>
+      <c r="I4">
+        <v>44</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>3.7853378054623861E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.75319999999999998</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.2467</v>
+      </c>
+      <c r="H5">
+        <v>137</v>
+      </c>
+      <c r="I5">
+        <v>77</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>6.5644465740297073E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>